<commit_message>
Updated designators on BOM, added a price for the TO220 mounting kit
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -92,18 +92,12 @@
     <t>31K8856</t>
   </si>
   <si>
-    <t>U1Mx</t>
-  </si>
-  <si>
     <t>Q1Mx</t>
   </si>
   <si>
     <t>Q2Mx</t>
   </si>
   <si>
-    <t>U$1</t>
-  </si>
-  <si>
     <t>TI</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
     <t>26K3586</t>
   </si>
   <si>
-    <t>Mates to U$1</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
@@ -204,6 +195,15 @@
   </si>
   <si>
     <t>94F4232</t>
+  </si>
+  <si>
+    <t>X$1</t>
+  </si>
+  <si>
+    <t>Mates to X$1</t>
+  </si>
+  <si>
+    <t>IC1Mx</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,22 +677,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H4" s="11">
         <v>7.0000000000000001E-3</v>
@@ -707,22 +707,22 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H5" s="11">
         <v>4.3999999999999997E-2</v>
@@ -737,28 +737,28 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
       </c>
       <c r="H6" s="11">
         <v>0.59</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -767,28 +767,28 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H7" s="11">
         <v>1.4E-2</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -797,28 +797,28 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="D8" t="s">
-        <v>32</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H8" s="11">
         <v>0.93899999999999995</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -827,13 +827,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E9" s="12">
         <v>4724</v>
@@ -842,7 +842,10 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>59</v>
+        <v>56</v>
+      </c>
+      <c r="H9" s="11">
+        <v>1.57</v>
       </c>
       <c r="J9" s="1"/>
     </row>
@@ -851,28 +854,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
         <v>41</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>44</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H10" s="11">
         <v>0.77400000000000002</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -881,28 +884,28 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="H11" s="11">
         <v>1.27</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -914,11 +917,11 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H13" s="11">
         <f>SUMPRODUCT(H2:H11,A2:A11)</f>
-        <v>14.916</v>
+        <v>27.476000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated BOM to source TLV431 from Newark
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Qty</t>
   </si>
@@ -104,9 +104,6 @@
     <t>TLV431CDBVR-Low-Voltage Adjustable Precision Shunt Regulator</t>
   </si>
   <si>
-    <t>TLV431CDBVR</t>
-  </si>
-  <si>
     <t>IC</t>
   </si>
   <si>
@@ -204,6 +201,12 @@
   </si>
   <si>
     <t>IC1Mx</t>
+  </si>
+  <si>
+    <t>76C8858</t>
+  </si>
+  <si>
+    <t>TLV431AIDBVR</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,22 +680,22 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="11">
         <v>7.0000000000000001E-3</v>
@@ -707,22 +710,22 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H5" s="11">
         <v>4.3999999999999997E-2</v>
@@ -740,25 +743,25 @@
         <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>26</v>
+      <c r="E6" t="s">
+        <v>60</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="H6" s="11">
-        <v>0.59</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -767,22 +770,22 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H7" s="11">
         <v>1.4E-2</v>
@@ -797,22 +800,22 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="11">
         <v>0.93899999999999995</v>
@@ -827,13 +830,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
       </c>
       <c r="E9" s="12">
         <v>4724</v>
@@ -842,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="11">
         <v>1.57</v>
@@ -854,28 +857,28 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
-      </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="11">
         <v>0.77400000000000002</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J10" s="1"/>
     </row>
@@ -884,28 +887,28 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="11">
         <v>1.27</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J11" s="1"/>
     </row>
@@ -917,11 +920,11 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H13" s="11">
         <f>SUMPRODUCT(H2:H11,A2:A11)</f>
-        <v>27.476000000000003</v>
+        <v>25.38</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added new parts to BoM (C1Mx, RA2Mx, RA3Mx)
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>Qty</t>
   </si>
@@ -65,12 +65,6 @@
     <t>R2Mx</t>
   </si>
   <si>
-    <t xml:space="preserve">RAx </t>
-  </si>
-  <si>
-    <t>RBx</t>
-  </si>
-  <si>
     <t>VISHAY DALE</t>
   </si>
   <si>
@@ -207,6 +201,39 @@
   </si>
   <si>
     <t>TLV431AIDBVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VISHAY </t>
+  </si>
+  <si>
+    <t>VJ0603Y104KXACW1BC</t>
+  </si>
+  <si>
+    <t>52X6485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RA1Mx </t>
+  </si>
+  <si>
+    <t>RBMx</t>
+  </si>
+  <si>
+    <t>C1Mx</t>
+  </si>
+  <si>
+    <t>Surface Mount Chip Resistor, Thick Film, AEC-Q200 CRCW Series, 2 Mohm, 100 mW, ± 1%, 75 V</t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitor, VJ.W1BC Series, 0.1 uF, 10%, X7R, 50 V, 0603 [1608 Metric]</t>
+  </si>
+  <si>
+    <t>CRCW06032M00FKEA</t>
+  </si>
+  <si>
+    <t>52K8249</t>
+  </si>
+  <si>
+    <t>RA2Mx, RA3Mx</t>
   </si>
 </sst>
 </file>
@@ -567,10 +594,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,22 +647,22 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="10">
         <v>3.0000000000000001E-3</v>
@@ -647,31 +674,31 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>67</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="11">
-        <v>8.9999999999999993E-3</v>
+        <v>68</v>
+      </c>
+      <c r="H3" s="10">
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -679,29 +706,29 @@
       <c r="A4" s="3">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
+      <c r="B4" t="s">
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>50</v>
+        <v>13</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>49</v>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
       <c r="H4" s="11">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>13</v>
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="J4" s="1"/>
     </row>
@@ -709,29 +736,29 @@
       <c r="A5" s="3">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
-        <v>44</v>
+      <c r="B5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>46</v>
-      </c>
       <c r="H5" s="11">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>14</v>
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -740,28 +767,28 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>60</v>
+        <v>43</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="H6" s="11">
-        <v>0.32800000000000001</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>58</v>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -770,28 +797,28 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="H7" s="11">
-        <v>1.4E-2</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>22</v>
+        <v>1.2E-2</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>64</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -800,28 +827,28 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>58</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="H8" s="11">
-        <v>0.93899999999999995</v>
+        <v>0.32800000000000001</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="J8" s="1"/>
     </row>
@@ -830,110 +857,170 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="12">
-        <v>4724</v>
+        <v>27</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="H9" s="11">
-        <v>1.57</v>
+        <v>1.4E-2</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>32</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H10" s="11">
-        <v>0.77400000000000002</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="12">
+        <v>4724</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="11">
+        <v>1.57</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" s="11">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="11">
+      <c r="F13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="11">
         <v>1.27</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="11">
-        <f>SUMPRODUCT(H2:H11,A2:A11)</f>
-        <v>25.38</v>
-      </c>
+      <c r="I13" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="11">
+        <f>SUMPRODUCT(H2:H13,A2:A13)</f>
+        <v>25.540000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated BoM with new part for C1Mx
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -203,15 +203,6 @@
     <t>TLV431AIDBVR</t>
   </si>
   <si>
-    <t xml:space="preserve">VISHAY </t>
-  </si>
-  <si>
-    <t>VJ0603Y104KXACW1BC</t>
-  </si>
-  <si>
-    <t>52X6485</t>
-  </si>
-  <si>
     <t xml:space="preserve">RA1Mx </t>
   </si>
   <si>
@@ -224,9 +215,6 @@
     <t>Surface Mount Chip Resistor, Thick Film, AEC-Q200 CRCW Series, 2 Mohm, 100 mW, ± 1%, 75 V</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitor, VJ.W1BC Series, 0.1 uF, 10%, X7R, 50 V, 0603 [1608 Metric]</t>
-  </si>
-  <si>
     <t>CRCW06032M00FKEA</t>
   </si>
   <si>
@@ -234,6 +222,18 @@
   </si>
   <si>
     <t>RA2Mx, RA3Mx</t>
+  </si>
+  <si>
+    <t>SMD Multilayer Ceramic Capacitor, GRM Series, 0.01 µF, ± 10%, X7R, 50 V, 0603 [1608 Metric]</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>GRM188R71H103KA01D</t>
+  </si>
+  <si>
+    <t>38K1669</t>
   </si>
 </sst>
 </file>
@@ -597,7 +597,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -686,19 +686,19 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H3" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -758,7 +758,7 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -788,7 +788,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J6" s="1"/>
     </row>
@@ -803,22 +803,22 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="11">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="H7" s="11">
-        <v>1.2E-2</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="J7" s="1"/>
     </row>
@@ -1011,7 +1011,7 @@
       </c>
       <c r="H15" s="11">
         <f>SUMPRODUCT(H2:H13,A2:A13)</f>
-        <v>25.540000000000003</v>
+        <v>25.507999999999999</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed vendor for D44VH10 transistor to Mouser because Newark is out of stock.
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" refMode="R1C1"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
   <si>
     <t>Qty</t>
   </si>
@@ -68,15 +68,9 @@
     <t>VISHAY DALE</t>
   </si>
   <si>
-    <t>19K7930</t>
-  </si>
-  <si>
     <t>Surface Mount Chip Resistor, Thick Film, AEC-Q200 CRCW Series, 1 kohm, 100 mW, ± 5%, 75 V</t>
   </si>
   <si>
-    <t>CRCW06031K00JNEA</t>
-  </si>
-  <si>
     <t>Surface Mount Chip Resistor, Thick Film, AEC-Q200 CRCW Series, 100 ohm, 100 mW, ± 5%, 75 V</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>D44VH10G</t>
   </si>
   <si>
-    <t>26K3586</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
@@ -234,6 +225,18 @@
   </si>
   <si>
     <t>38K1669</t>
+  </si>
+  <si>
+    <t>07H2487</t>
+  </si>
+  <si>
+    <t>CRCW06031K00JNEB</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>863-D44VH10G</t>
   </si>
 </sst>
 </file>
@@ -281,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -313,6 +316,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,10 +604,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,12 +618,13 @@
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,13 +652,14 @@
       <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>9</v>
@@ -655,14 +667,14 @@
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>16</v>
+      <c r="E2" t="s">
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
+      <c r="G2" t="s">
+        <v>67</v>
       </c>
       <c r="H2" s="10">
         <v>3.0000000000000001E-3</v>
@@ -670,14 +682,15 @@
       <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="14"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
@@ -686,28 +699,29 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H3" s="10">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="J3" s="14"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>9</v>
@@ -716,13 +730,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H4" s="11">
         <v>8.9999999999999993E-3</v>
@@ -730,200 +744,207 @@
       <c r="I4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="14"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H5" s="11">
-        <v>7.0000000000000001E-3</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="J5" s="14"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="11">
         <v>4.3999999999999997E-2</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="J6" s="14"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H7" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H8" s="11">
         <v>0.32800000000000001</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J8" s="14"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H9" s="11">
         <v>1.4E-2</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="H10" s="11">
-        <v>0.93899999999999995</v>
+        <v>0.98</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E11" s="12">
         <v>4724</v>
@@ -932,87 +953,91 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H11" s="11">
         <v>1.57</v>
       </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J11" s="14"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H12" s="11">
         <v>0.77400000000000002</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="J12" s="14"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H13" s="11">
         <v>1.27</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="J13" s="14"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="C14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H15" s="11">
         <f>SUMPRODUCT(H2:H13,A2:A13)</f>
-        <v>25.507999999999999</v>
-      </c>
+        <v>26.34</v>
+      </c>
+      <c r="K15" s="11"/>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" s="3"/>

</xml_diff>